<commit_message>
add orders list on user home page
</commit_message>
<xml_diff>
--- a/passwords/passwords.xlsx
+++ b/passwords/passwords.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>email</t>
   </si>
@@ -53,6 +52,9 @@
   </si>
   <si>
     <t>PasswordUser</t>
+  </si>
+  <si>
+    <t>6f42205f20666a04d1f2ee777a799c383d4af4be593eb607b0f1cda06bc73c50</t>
   </si>
 </sst>
 </file>
@@ -405,7 +407,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -466,6 +468,9 @@
       <c r="B5" t="s">
         <v>11</v>
       </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>